<commit_message>
let the testing begin
</commit_message>
<xml_diff>
--- a/IndustrySmartware/components.xlsx
+++ b/IndustrySmartware/components.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>β (Hr)</t>
   </si>
@@ -843,13 +843,46 @@
   </si>
   <si>
     <t>UNSKILLED</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1018,9 +1051,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1032,7 +1065,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1041,64 +1074,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1447,33 +1483,33 @@
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="24"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="19" t="s">
         <v>25</v>
       </c>
@@ -1482,20 +1518,20 @@
         <v>26</v>
       </c>
       <c r="I2" s="19"/>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>28</v>
       </c>
       <c r="L2" s="19"/>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="18" t="s">
         <v>21</v>
       </c>
       <c r="R2" s="19" t="s">
@@ -1506,7 +1542,7 @@
         <v>26</v>
       </c>
       <c r="U2" s="19"/>
-      <c r="V2" s="17" t="s">
+      <c r="V2" s="18" t="s">
         <v>27</v>
       </c>
       <c r="W2" s="19" t="s">
@@ -1515,74 +1551,74 @@
       <c r="X2" s="19"/>
     </row>
     <row r="3" spans="1:24" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="20" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="22"/>
       <c r="F3" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="19"/>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17" t="s">
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="20" t="s">
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="21"/>
-      <c r="T3" s="17" t="s">
+      <c r="S3" s="22"/>
+      <c r="T3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17" t="s">
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="17" t="s">
+      <c r="X3" s="18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
     </row>
     <row r="5" spans="1:24" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="10" t="s">
         <v>34</v>
       </c>
@@ -1613,8 +1649,8 @@
       <c r="L5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
       <c r="Q5" s="10" t="s">
         <v>34</v>
       </c>
@@ -1641,7 +1677,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1675,7 +1711,7 @@
         <v>10000</v>
       </c>
       <c r="L6" s="6"/>
-      <c r="O6" s="17" t="s">
+      <c r="O6" s="18" t="s">
         <v>42</v>
       </c>
       <c r="P6" s="1" t="s">
@@ -1705,7 +1741,7 @@
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
@@ -1737,7 +1773,7 @@
         <v>9000</v>
       </c>
       <c r="L7" s="6"/>
-      <c r="O7" s="17"/>
+      <c r="O7" s="18"/>
       <c r="P7" s="1" t="s">
         <v>44</v>
       </c>
@@ -1765,7 +1801,7 @@
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1797,7 +1833,7 @@
         <v>9500</v>
       </c>
       <c r="L8" s="6"/>
-      <c r="O8" s="17"/>
+      <c r="O8" s="18"/>
       <c r="P8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1825,7 +1861,7 @@
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
@@ -1857,7 +1893,7 @@
         <v>10000</v>
       </c>
       <c r="L9" s="6"/>
-      <c r="O9" s="17"/>
+      <c r="O9" s="18"/>
       <c r="P9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2065,7 +2101,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2099,7 +2135,7 @@
         <v>9000</v>
       </c>
       <c r="L13" s="6"/>
-      <c r="O13" s="17" t="s">
+      <c r="O13" s="18" t="s">
         <v>50</v>
       </c>
       <c r="P13" s="1" t="s">
@@ -2129,7 +2165,7 @@
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="1" t="s">
         <v>52</v>
       </c>
@@ -2161,7 +2197,7 @@
         <v>10000</v>
       </c>
       <c r="L14" s="6"/>
-      <c r="O14" s="17"/>
+      <c r="O14" s="18"/>
       <c r="P14" s="1" t="s">
         <v>52</v>
       </c>
@@ -2189,7 +2225,7 @@
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="1" t="s">
         <v>53</v>
       </c>
@@ -2221,7 +2257,7 @@
         <v>9000</v>
       </c>
       <c r="L15" s="6"/>
-      <c r="O15" s="17"/>
+      <c r="O15" s="18"/>
       <c r="P15" s="1" t="s">
         <v>53</v>
       </c>
@@ -2249,7 +2285,7 @@
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2281,7 +2317,7 @@
         <v>9500</v>
       </c>
       <c r="L16" s="6"/>
-      <c r="O16" s="17"/>
+      <c r="O16" s="18"/>
       <c r="P16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2309,7 +2345,7 @@
       <c r="X16" s="2"/>
     </row>
     <row r="17" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
@@ -2341,7 +2377,7 @@
         <v>10000</v>
       </c>
       <c r="L17" s="6"/>
-      <c r="O17" s="17"/>
+      <c r="O17" s="18"/>
       <c r="P17" s="1" t="s">
         <v>55</v>
       </c>
@@ -2369,7 +2405,7 @@
       <c r="X17" s="2"/>
     </row>
     <row r="18" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
@@ -2401,7 +2437,7 @@
         <v>10000</v>
       </c>
       <c r="L18" s="6"/>
-      <c r="O18" s="18"/>
+      <c r="O18" s="25"/>
       <c r="P18" s="1" t="s">
         <v>56</v>
       </c>
@@ -2429,7 +2465,7 @@
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="1" t="s">
         <v>57</v>
       </c>
@@ -2461,7 +2497,7 @@
         <v>9000</v>
       </c>
       <c r="L19" s="6"/>
-      <c r="O19" s="18"/>
+      <c r="O19" s="25"/>
       <c r="P19" s="1" t="s">
         <v>57</v>
       </c>
@@ -2490,16 +2526,16 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="O1:X1"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T3:U4"/>
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="R3:S4"/>
+    <mergeCell ref="O6:O9"/>
+    <mergeCell ref="O13:O17"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D3:E4"/>
     <mergeCell ref="F3:G4"/>
@@ -2511,17 +2547,17 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I4"/>
+    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="O1:X1"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T3:U4"/>
+    <mergeCell ref="P2:P5"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="R3:S4"/>
     <mergeCell ref="O2:O5"/>
-    <mergeCell ref="O6:O9"/>
-    <mergeCell ref="O13:O17"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2533,7 +2569,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,8 +2591,8 @@
       <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="19" t="s">
         <v>70</v>
       </c>
@@ -2575,14 +2611,14 @@
         <v>20</v>
       </c>
       <c r="B3" s="19"/>
-      <c r="C3" s="28">
+      <c r="C3" s="26">
         <v>800</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28">
+      <c r="D3" s="26"/>
+      <c r="E3" s="26">
         <v>500</v>
       </c>
-      <c r="F3" s="28"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="27">
         <v>300</v>
       </c>
@@ -2593,18 +2629,18 @@
         <v>66</v>
       </c>
       <c r="B4" s="19"/>
-      <c r="C4" s="28">
-        <v>2</v>
-      </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28">
+      <c r="C4" s="26">
+        <v>2</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26">
         <v>4</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28">
+      <c r="F4" s="26"/>
+      <c r="G4" s="26">
         <v>8</v>
       </c>
-      <c r="H4" s="28"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2633,7 +2669,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -2659,7 +2695,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -2683,7 +2719,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -2707,7 +2743,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -2734,7 +2770,9 @@
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="17" t="s">
+        <v>73</v>
+      </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
@@ -2758,7 +2796,9 @@
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="17" t="s">
+        <v>7</v>
+      </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
@@ -2782,7 +2822,9 @@
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="17" t="s">
+        <v>8</v>
+      </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
@@ -2803,7 +2845,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2829,7 +2871,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2853,7 +2895,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
@@ -2877,7 +2919,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
@@ -2901,7 +2943,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
@@ -2925,7 +2967,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="4" t="s">
         <v>15</v>
       </c>
@@ -2949,7 +2991,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="4" t="s">
         <v>16</v>
       </c>
@@ -2973,23 +3015,29 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25" t="s">
+      <c r="B20" s="28"/>
+      <c r="C20" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25" t="s">
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C4:D4"/>
@@ -3003,12 +3051,6 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>